<commit_message>
Ajustes de mensaje d erespuesta
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/svp-rediseno-personas-web-tests-bdd-screenplay/SVP/src/test/resources/datadriven/registrarusuario/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Todo1\Automatizacion\svp-rediseno-personas-web-tests-bdd-screenplay\SVP\src\test\resources\datadriven\registrarusuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,18 +17,18 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Orientacion</t>
   </si>
@@ -82,13 +82,34 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>¡Registro exitoso!</t>
+  </si>
+  <si>
+    <t>Registro de usuario incorrecto</t>
+  </si>
+  <si>
+    <t>mensajeRespuesta</t>
+  </si>
+  <si>
+    <t>¡Lo Sentimos!</t>
+  </si>
+  <si>
+    <t>Ingresa otro usuario. El que ingresaste ya esta en uso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>informativo para realizar el registro nuevamente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -145,11 +166,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -162,6 +194,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,27 +511,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -527,8 +563,11 @@
       <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -543,8 +582,11 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -559,8 +601,11 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -575,8 +620,11 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -591,8 +639,11 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -607,6 +658,14 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -632,19 +691,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Ajustes a mensajes de respuesta registro
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="Listas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,9 +99,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>informativo para realizar el registro nuevamente</t>
-  </si>
-  <si>
     <t>correoElectronico</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>¡Registro exitoso!</t>
+  </si>
+  <si>
+    <t>Para continuar debes registrarte de nuevo en la aplicación.</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -572,7 +572,7 @@
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -607,13 +607,13 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>19</v>
@@ -630,10 +630,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -643,16 +643,16 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -696,7 +696,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -717,7 +717,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="9"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="9" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajustes a registro de usuario
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Orientacion</t>
   </si>
@@ -84,18 +84,12 @@
     <t>5</t>
   </si>
   <si>
-    <t>Registro de usuario incorrecto</t>
-  </si>
-  <si>
     <t>mensajeRespuesta</t>
   </si>
   <si>
     <t>¡Lo Sentimos!</t>
   </si>
   <si>
-    <t>Ingresa otro usuario. El que ingresaste ya esta en uso</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>hola</t>
   </si>
   <si>
-    <t>25130103</t>
-  </si>
-  <si>
     <t>3182314777</t>
   </si>
   <si>
@@ -132,7 +123,13 @@
     <t>OSVPPRU01</t>
   </si>
   <si>
-    <t>OSVPPRU80</t>
+    <t>Ingresa otro usuario. El que ingresaste ya está en uso</t>
+  </si>
+  <si>
+    <t>OSVPPRU99</t>
+  </si>
+  <si>
+    <t>396000297</t>
   </si>
 </sst>
 </file>
@@ -567,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -622,19 +619,19 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="N1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -648,10 +645,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -661,16 +658,16 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>7</v>
@@ -687,10 +684,10 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
@@ -700,18 +697,18 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="9" t="s">
+      <c r="N3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -726,10 +723,10 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1">
         <v>1234</v>
@@ -739,18 +736,18 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -765,10 +762,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -778,68 +775,36 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="4" t="s">
+      <c r="N5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1234</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1234</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="4" t="s">
+    </row>
+    <row r="10" spans="1:15">
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="G11" s="10"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="10"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="N13" t="s">
         <v>20</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="G12" s="10"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="N14" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -848,10 +813,9 @@
     <hyperlink ref="K3" r:id="rId2"/>
     <hyperlink ref="K4" r:id="rId3"/>
     <hyperlink ref="K5" r:id="rId4"/>
-    <hyperlink ref="K6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="597" r:id="rId6"/>
+  <pageSetup orientation="portrait" verticalDpi="597" r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -859,7 +823,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B6</xm:sqref>
+          <xm:sqref>B2:B5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Ajuste de orden de excenarios para utilidad de data
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
@@ -564,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -639,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -648,7 +648,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -667,7 +667,7 @@
         <v>25</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>7</v>
@@ -687,7 +687,7 @@
         <v>33</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
@@ -705,10 +705,10 @@
       <c r="M3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="4" t="s">
+      <c r="N3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -744,11 +744,11 @@
       <c r="M4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>7</v>
+      <c r="N4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -756,7 +756,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -765,7 +765,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -784,35 +784,35 @@
         <v>25</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="G11" s="10"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="10"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="N13" t="s">
+      <c r="N12" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
-    <hyperlink ref="K4" r:id="rId3"/>
-    <hyperlink ref="K5" r:id="rId4"/>
+    <hyperlink ref="K5" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId2"/>
+    <hyperlink ref="K3" r:id="rId3"/>
+    <hyperlink ref="K4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="597" r:id="rId5"/>

</xml_diff>

<commit_message>
Ajustes a flujos y data
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
@@ -129,7 +129,7 @@
     <t>OSVPPRU99</t>
   </si>
   <si>
-    <t>396000297</t>
+    <t>1245123881</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Ajustes sonar y parametro de intentos en registro
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Orientacion</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
   <si>
     <t>mensajeRespuesta</t>
@@ -566,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -619,19 +616,19 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -645,10 +642,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -658,16 +655,16 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>7</v>
@@ -684,10 +681,10 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
@@ -697,16 +694,16 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>7</v>
@@ -723,10 +720,10 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1">
         <v>1234</v>
@@ -736,19 +733,19 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -762,10 +759,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -775,16 +772,16 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>7</v>
@@ -804,7 +801,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="N12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste para pull request
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
+++ b/SVP/src/test/resources/datadriven/registrarusuario/registrar_usuario.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Orientacion</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Para continuar debes registrarte de nuevo en la aplicación.</t>
-  </si>
-  <si>
-    <t>intentos</t>
   </si>
   <si>
     <t>OSVPPRU01</t>
@@ -564,7 +561,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -582,9 +579,10 @@
     <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="15.140625" customWidth="1"/>
     <col min="14" max="14" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -627,11 +625,8 @@
       <c r="N1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -642,10 +637,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1">
         <v>1234</v>
@@ -666,11 +661,8 @@
       <c r="N2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -681,10 +673,10 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="1">
         <v>1234</v>
@@ -703,13 +695,10 @@
         <v>24</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -720,10 +709,10 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="1">
         <v>1234</v>
@@ -744,11 +733,8 @@
       <c r="N4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -759,10 +745,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -783,23 +769,20 @@
       <c r="N5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+    </row>
+    <row r="9" spans="1:14">
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:14">
       <c r="G10" s="10"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:14">
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:14">
       <c r="N12" t="s">
         <v>19</v>
       </c>

</xml_diff>